<commit_message>
FINAL DOCUMENTACION 1A PARTE
</commit_message>
<xml_diff>
--- a/Docs/DocumentacionEscenarioPruebas.xlsx
+++ b/Docs/DocumentacionEscenarioPruebas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>SENTENCIA SQL</t>
   </si>
@@ -132,6 +132,21 @@
 UNION ALL SELECT CEDULA, NOMBRE, ROL, EMAIL FROM (PEDIDO NATURAL JOIN PEDIDOPRODUCTO) NATURAL JOIN USUARIO
 WHERE CEDULA not IN (SELECT CEDULA FROM (PEDIDO NATURAL JOIN PEDIDOMENU) NATURAL JOIN USUARIO CEDULA )
 GROUP BY CEDULA, NOMBRE, EMAIL, ROL ;</t>
+  </si>
+  <si>
+    <t>En este caso los valores que entran por parametros son el ROL (usuario), el local del restaurante, el producto del determinado restaurante y los rangos de fechas. Estos resultados varían según todos menos el rol, ya que esta tiene que ser una constante debido a lo requerido. Por otra parte, la respuesta se agrandaría si el rango de fechas es mayor, sin embargo, lo que más determina este tamaño de respuesta es el producto y el restaurante ingresados.</t>
+  </si>
+  <si>
+    <t>La distribución de los datos de entrada se estima uniforme para cada producto de cada restaurante, puesto que al tener en cuenta el tamaño de las tablas de los productos, de los restaurantes y de los pedidos, es bastante poco probable que más de un cliente hayan consumido lo mismo en el mismo rango de fechas.</t>
+  </si>
+  <si>
+    <t>La distribución de los parámetros de entrada en este requerimiento esta determinada gracias a los pedidos, ya que en ellos y la cantidada de veces que un producto haga parte de una de estas tuplas es donde se ve realmente la cardinalidad.</t>
+  </si>
+  <si>
+    <t>Los parámetros de entrada en este caso es el costo de 1.5 SMDV solamente, puesto que el resto se toma como una constante que se da gracias a este valor de entrada.</t>
+  </si>
+  <si>
+    <t>La distribución de los parámetros de entrada en este requerimiento esta determinada gracias a los pedidos, ya que en ellos se puede determinar los mejores clientes, lo que pidieron, cuando lo pidieron, el costo de lo que pidieron  y cada cuanto lo pidieron.</t>
   </si>
 </sst>
 </file>
@@ -1193,6 +1208,256 @@
         <a:xfrm>
           <a:off x="18051780" y="10759441"/>
           <a:ext cx="7612380" cy="3223260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7627620</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3863340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC18E26-08A6-4D14-8947-82C44C550012}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18074640" y="14043660"/>
+          <a:ext cx="7604760" cy="3832860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D27A6FAD-BF13-4BE9-A3DC-F58C7AE190DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18105120" y="17937480"/>
+          <a:ext cx="7650480" cy="2537460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagen 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1EDF950-2346-4CC6-8770-54B276EF0D35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18135600" y="20505420"/>
+          <a:ext cx="7650480" cy="2537460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2552700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagen 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{044C118E-DEE4-45FC-922B-F710870E2FF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18112740" y="23050500"/>
+          <a:ext cx="7650480" cy="2537460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2537460</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagen 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{915C8A58-53CF-45B4-B128-B172282982BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18097500" y="25626060"/>
+          <a:ext cx="7650480" cy="2537460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1503,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495592F4-0ED0-44AA-A160-5F1BDEECFE03}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,10 +1872,14 @@
       <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="306.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1620,10 +1889,14 @@
       <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="202.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1633,29 +1906,53 @@
       <c r="C8" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="204" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
@@ -1667,6 +1964,12 @@
       </c>
       <c r="C12" s="10" t="s">
         <v>27</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>